<commit_message>
Added predictor by seeds
</commit_message>
<xml_diff>
--- a/ExperimentsResults.xlsx
+++ b/ExperimentsResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>EloPP V1, Scores 1 or 0</t>
   </si>
@@ -51,16 +51,39 @@
   </si>
   <si>
     <t>EloPP V1, Scores Logistic, Regularization = 0.25</t>
+  </si>
+  <si>
+    <t>EloPP V1, Scores Logistic, Regularization = calibrated = 0.22</t>
+  </si>
+  <si>
+    <t>TeamSeedPredictor</t>
+  </si>
+  <si>
+    <t>EloPP V1, Scores Logistic, Regularization = calibrated = 0.22, RandomSeed=421</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -73,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,11 +105,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -109,18 +142,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="3" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +478,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>0.57126994187589597</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.41522680074534302</v>
       </c>
     </row>
@@ -506,6 +560,30 @@
       </c>
       <c r="C9">
         <v>0.40655339765626197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.40623008569885799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.408240672723793</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.406812534700287</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactoring, home adv calibration
</commit_message>
<xml_diff>
--- a/ExperimentsResults.xlsx
+++ b/ExperimentsResults.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>EloPP V1, Scores 1 or 0</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>EloPP V1, HomeAdvantage - 0.3</t>
+  </si>
+  <si>
+    <t>Elopp V1, 200 iterations, Reg=0.2256</t>
+  </si>
+  <si>
+    <t>Elopp V1, 200 iterations, Reg=0.2256, RandomSeed=421</t>
+  </si>
+  <si>
+    <t>Elopp V1, 400 iterations, Reg=0.2256</t>
+  </si>
+  <si>
+    <t>Elopp V1, 400 iterations, Reg=0.2256, RandomSeed=421</t>
+  </si>
+  <si>
+    <t>Elopp V1, 600 iterations, Reg=0.2256, RandomSeed=421</t>
+  </si>
+  <si>
+    <t>Elopp V1, 600 iterations, Reg=0.2256, RandomSeed=42</t>
+  </si>
+  <si>
+    <t>Elopp V1, 50 iterations, Reg=0.2256, RandomSeed=42, HomeAdv=0.27</t>
+  </si>
+  <si>
+    <t>Elopp V1, 600 iterations, Reg=0.2256, RandomSeed=42, HomeAdv=0.27</t>
+  </si>
+  <si>
+    <t>Elopp V1, 100 iterations, Reg=0.2256, RandomSeed=42, HomeAdv=-0.0105</t>
+  </si>
+  <si>
+    <t>Elopp V1, 600 iterations, Reg=0.2256, RandomSeed=42, HomeAdv=-0.0105</t>
   </si>
 </sst>
 </file>
@@ -470,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:C13"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,6 +614,9 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
+      <c r="B10">
+        <v>0.54894211041483298</v>
+      </c>
       <c r="C10" s="1">
         <v>0.40623008569885799</v>
       </c>
@@ -592,6 +625,9 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
+      <c r="B11">
+        <v>0.55229771608690903</v>
+      </c>
       <c r="C11" s="4">
         <v>0.408240672723793</v>
       </c>
@@ -600,6 +636,9 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
+      <c r="B12">
+        <v>0.55010864533221904</v>
+      </c>
       <c r="C12" s="3">
         <v>0.406812534700287</v>
       </c>
@@ -609,10 +648,120 @@
         <v>12</v>
       </c>
       <c r="B13">
+        <v>0.54667524152360103</v>
+      </c>
+      <c r="C13">
         <v>0.40581239595836999</v>
       </c>
-      <c r="C13">
-        <v>0.54667524152360103</v>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.548950207783092</v>
+      </c>
+      <c r="C14">
+        <v>0.406200483828216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.54946373351655198</v>
+      </c>
+      <c r="C15">
+        <v>0.40645411249053998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>0.54991849851126096</v>
+      </c>
+      <c r="C16">
+        <v>0.40667455430965399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>0.54979899562884904</v>
+      </c>
+      <c r="C17">
+        <v>0.406682990358605</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>0.54974746327577895</v>
+      </c>
+      <c r="C18">
+        <v>0.40660637354100199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.55000381802544596</v>
+      </c>
+      <c r="C19">
+        <v>0.40675764731547498</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>0.54927045457164503</v>
+      </c>
+      <c r="C20">
+        <v>0.406341446076118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>0.55033822326860404</v>
+      </c>
+      <c r="C21">
+        <v>0.40681785132455101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>0.54932030697169598</v>
+      </c>
+      <c r="C22">
+        <v>0.406441315044622</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>0.54984822782609899</v>
+      </c>
+      <c r="C23">
+        <v>0.40670593687463802</v>
       </c>
     </row>
   </sheetData>

</xml_diff>